<commit_message>
Train the model for SVM
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lowcodemindstech-my.sharepoint.com/personal/kawisha_nilmani_lowcodeminds_com/Documents/Desktop/Automate email classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_430591B4D3D05B37E73A3511595ED87656CD2BB3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB14A2B1-D87C-4254-994A-E33AE073E909}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_430591B4D3D05B37E73A3511595ED87656CD2BB3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D33977-DA2C-4342-A8AB-F05E0EAC44EE}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="140">
   <si>
     <t>Email ID</t>
   </si>
@@ -428,6 +428,18 @@
   </si>
   <si>
     <t>Hi, I just need to add another property to my insurance policy. What are the steps to do.</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
+    <t>Automobile</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -790,17 +802,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.28515625" customWidth="1"/>
     <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,10 +824,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -819,10 +838,13 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -830,10 +852,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -841,10 +866,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -852,10 +880,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -863,10 +894,13 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -874,10 +908,13 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -885,10 +922,13 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -896,10 +936,13 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -907,10 +950,13 @@
         <v>27</v>
       </c>
       <c r="C10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -918,10 +964,13 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
+        <v>138</v>
+      </c>
+      <c r="D11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -929,10 +978,13 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -940,10 +992,13 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -951,10 +1006,13 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -962,10 +1020,13 @@
         <v>41</v>
       </c>
       <c r="C15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -973,10 +1034,13 @@
         <v>43</v>
       </c>
       <c r="C16" t="s">
+        <v>137</v>
+      </c>
+      <c r="D16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -984,10 +1048,13 @@
         <v>45</v>
       </c>
       <c r="C17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -995,10 +1062,13 @@
         <v>48</v>
       </c>
       <c r="C18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1006,10 +1076,13 @@
         <v>50</v>
       </c>
       <c r="C19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1017,10 +1090,13 @@
         <v>52</v>
       </c>
       <c r="C20" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -1028,10 +1104,13 @@
         <v>54</v>
       </c>
       <c r="C21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1039,10 +1118,13 @@
         <v>56</v>
       </c>
       <c r="C22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1050,10 +1132,13 @@
         <v>58</v>
       </c>
       <c r="C23" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1061,10 +1146,13 @@
         <v>60</v>
       </c>
       <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1072,10 +1160,13 @@
         <v>62</v>
       </c>
       <c r="C25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1083,10 +1174,13 @@
         <v>64</v>
       </c>
       <c r="C26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1094,10 +1188,13 @@
         <v>66</v>
       </c>
       <c r="C27" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -1105,10 +1202,13 @@
         <v>68</v>
       </c>
       <c r="C28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -1116,10 +1216,13 @@
         <v>70</v>
       </c>
       <c r="C29" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -1127,10 +1230,13 @@
         <v>72</v>
       </c>
       <c r="C30" t="s">
+        <v>136</v>
+      </c>
+      <c r="D30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1138,10 +1244,13 @@
         <v>74</v>
       </c>
       <c r="C31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D31" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1149,10 +1258,13 @@
         <v>76</v>
       </c>
       <c r="C32" t="s">
+        <v>138</v>
+      </c>
+      <c r="D32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>40</v>
       </c>
@@ -1160,10 +1272,13 @@
         <v>78</v>
       </c>
       <c r="C33" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1171,10 +1286,13 @@
         <v>80</v>
       </c>
       <c r="C34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1182,10 +1300,13 @@
         <v>82</v>
       </c>
       <c r="C35" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -1193,10 +1314,13 @@
         <v>84</v>
       </c>
       <c r="C36" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1204,10 +1328,13 @@
         <v>86</v>
       </c>
       <c r="C37" t="s">
+        <v>136</v>
+      </c>
+      <c r="D37" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>20</v>
       </c>
@@ -1215,10 +1342,13 @@
         <v>88</v>
       </c>
       <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1226,10 +1356,13 @@
         <v>90</v>
       </c>
       <c r="C39" t="s">
+        <v>137</v>
+      </c>
+      <c r="D39" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1237,10 +1370,13 @@
         <v>92</v>
       </c>
       <c r="C40" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1248,10 +1384,13 @@
         <v>94</v>
       </c>
       <c r="C41" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1259,10 +1398,13 @@
         <v>96</v>
       </c>
       <c r="C42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>35</v>
       </c>
@@ -1270,10 +1412,13 @@
         <v>98</v>
       </c>
       <c r="C43" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -1281,10 +1426,13 @@
         <v>100</v>
       </c>
       <c r="C44" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -1292,10 +1440,13 @@
         <v>102</v>
       </c>
       <c r="C45" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>29</v>
       </c>
@@ -1303,10 +1454,13 @@
         <v>104</v>
       </c>
       <c r="C46" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>106</v>
       </c>
@@ -1314,10 +1468,13 @@
         <v>107</v>
       </c>
       <c r="C47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1325,10 +1482,13 @@
         <v>109</v>
       </c>
       <c r="C48" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>32</v>
       </c>
@@ -1336,10 +1496,13 @@
         <v>111</v>
       </c>
       <c r="C49" t="s">
+        <v>136</v>
+      </c>
+      <c r="D49" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -1347,10 +1510,13 @@
         <v>114</v>
       </c>
       <c r="C50" t="s">
+        <v>137</v>
+      </c>
+      <c r="D50" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -1358,10 +1524,13 @@
         <v>116</v>
       </c>
       <c r="C51" t="s">
+        <v>136</v>
+      </c>
+      <c r="D51" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -1369,10 +1538,13 @@
         <v>118</v>
       </c>
       <c r="C52" t="s">
+        <v>137</v>
+      </c>
+      <c r="D52" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>106</v>
       </c>
@@ -1380,10 +1552,13 @@
         <v>120</v>
       </c>
       <c r="C53" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>113</v>
       </c>
@@ -1391,10 +1566,13 @@
         <v>121</v>
       </c>
       <c r="C54" t="s">
+        <v>136</v>
+      </c>
+      <c r="D54" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>3</v>
       </c>
@@ -1402,10 +1580,13 @@
         <v>123</v>
       </c>
       <c r="C55" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>125</v>
       </c>
@@ -1413,10 +1594,13 @@
         <v>126</v>
       </c>
       <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>125</v>
       </c>
@@ -1424,10 +1608,13 @@
         <v>128</v>
       </c>
       <c r="C57" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>113</v>
       </c>
@@ -1435,10 +1622,13 @@
         <v>78</v>
       </c>
       <c r="C58" t="s">
+        <v>136</v>
+      </c>
+      <c r="D58" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>32</v>
       </c>
@@ -1446,10 +1636,13 @@
         <v>131</v>
       </c>
       <c r="C59" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>106</v>
       </c>
@@ -1457,10 +1650,13 @@
         <v>133</v>
       </c>
       <c r="C60" t="s">
+        <v>136</v>
+      </c>
+      <c r="D60" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>3</v>
       </c>
@@ -1468,6 +1664,9 @@
         <v>134</v>
       </c>
       <c r="C61" t="s">
+        <v>137</v>
+      </c>
+      <c r="D61" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified emails excel file
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lowcodemindstech-my.sharepoint.com/personal/kawisha_nilmani_lowcodeminds_com/Documents/Desktop/Automate email classification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Lowcode Minds Technology Pvt Ltd\Desktop\Automate-Email-Classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="11_430591B4D3D05B37E73A3511595ED87656CD2BB3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{44D33977-DA2C-4342-A8AB-F05E0EAC44EE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362716C9-F064-4187-BD89-BE767B52F01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -804,7 +804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>

</xml_diff>